<commit_message>
changes in json and roundabout handling
</commit_message>
<xml_diff>
--- a/edfrs.xlsx
+++ b/edfrs.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Accidents" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="junction road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="roundabout road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,308 +525,1061 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:12</t>
+          <t>2024-09-05 16:26:12</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>43.53328715486533</v>
+        <v>42.97417332260869</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>33.84752639549302</v>
+        <v>44.58107609444188</v>
       </c>
       <c r="E2" t="n">
-        <v>47.96121177874241</v>
+        <v>52.46090207503978</v>
       </c>
       <c r="F2" t="n">
-        <v>41.3527495158252</v>
+        <v>46.25478479037855</v>
       </c>
       <c r="G2" t="n">
-        <v>56.79163337076277</v>
+        <v>33.2882515768774</v>
       </c>
       <c r="H2" t="n">
-        <v>37.71331471350325</v>
+        <v>38.28585207630584</v>
       </c>
       <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:14</t>
+          <t>2024-09-05 16:26:14</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42.36283881747845</v>
+        <v>42.67481608487603</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>43.93618808092773</v>
+        <v>36.12939588200859</v>
       </c>
       <c r="E3" t="n">
-        <v>45.9424491845229</v>
+        <v>44.14291941385915</v>
       </c>
       <c r="F3" t="n">
-        <v>43.61640675948694</v>
+        <v>48.86477250923694</v>
       </c>
       <c r="G3" t="n">
-        <v>38.30091210009538</v>
+        <v>33.2882515768774</v>
       </c>
       <c r="H3" t="n">
-        <v>40.83162800564008</v>
-      </c>
-      <c r="I3" t="n">
-        <v>42.30940799436627</v>
-      </c>
+        <v>46.2554587883988</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:16</t>
+          <t>2024-09-05 16:26:16</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.04662437316339</v>
+        <v>43.96354224852487</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>39.73335127168806</v>
+        <v>43.51201253375351</v>
       </c>
       <c r="E4" t="n">
-        <v>45.95404979242193</v>
+        <v>44.14291941385915</v>
       </c>
       <c r="F4" t="n">
-        <v>43.4140372154959</v>
+        <v>48.84141220800414</v>
       </c>
       <c r="G4" t="n">
-        <v>18.18163359309197</v>
+        <v>35.23568573173995</v>
       </c>
       <c r="H4" t="n">
-        <v>40.81865818251765</v>
+        <v>46.00108393599726</v>
       </c>
       <c r="I4" t="n">
-        <v>42.30940799436627</v>
+        <v>46.09519539959311</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:18</t>
+          <t>2024-09-05 16:26:18</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>37.53113683917073</v>
+        <v>43.43615874619285</v>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>35.17191485605005</v>
+        <v>33.63596365762184</v>
       </c>
       <c r="E5" t="n">
-        <v>43.58277235297811</v>
+        <v>45.15665799394298</v>
       </c>
       <c r="F5" t="n">
-        <v>43.1615899692099</v>
+        <v>46.77149055238785</v>
       </c>
       <c r="G5" t="n">
-        <v>24.99864014932926</v>
+        <v>35.21913314428828</v>
       </c>
       <c r="H5" t="n">
-        <v>38.36160248884758</v>
+        <v>45.12695363650936</v>
       </c>
       <c r="I5" t="n">
-        <v>42.30940799436627</v>
+        <v>46.09519539959311</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:20</t>
+          <t>2024-09-05 16:26:20</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35.88613365613747</v>
+        <v>43.75171533061922</v>
       </c>
       <c r="C6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="n">
-        <v>35.57081256157377</v>
+        <v>36.99999999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>43.5737103528761</v>
+        <v>45.08137348413874</v>
       </c>
       <c r="F6" t="n">
-        <v>29.39213939021401</v>
+        <v>46.65791259620053</v>
       </c>
       <c r="G6" t="n">
-        <v>30.63587815998829</v>
+        <v>39.32317305523195</v>
       </c>
       <c r="H6" t="n">
-        <v>38.11703636995895</v>
+        <v>44.68556497789069</v>
       </c>
       <c r="I6" t="n">
-        <v>42.30940799436627</v>
+        <v>44.09580535302485</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:22</t>
+          <t>2024-09-05 16:26:22</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>39.46276248888501</v>
+        <v>43.33090316646683</v>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="n">
-        <v>36.02873889110673</v>
+        <v>45.44526039925524</v>
       </c>
       <c r="E7" t="n">
-        <v>44.01032999886196</v>
+        <v>41.34625521007478</v>
       </c>
       <c r="F7" t="n">
-        <v>39.28687495112917</v>
+        <v>44.42916233957561</v>
       </c>
       <c r="G7" t="n">
-        <v>35.66434750411165</v>
+        <v>40.67849322010458</v>
       </c>
       <c r="H7" t="n">
-        <v>40.75335382340064</v>
+        <v>44.62150506643773</v>
       </c>
       <c r="I7" t="n">
-        <v>42.30940799436627</v>
+        <v>44.82742617074356</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:24</t>
+          <t>2024-09-05 16:26:24</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30.45954636676505</v>
+        <v>42.71502376175098</v>
       </c>
       <c r="C8" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n">
-        <v>29.90419354446533</v>
+        <v>36.2569852457465</v>
       </c>
       <c r="E8" t="n">
-        <v>33.68531287523405</v>
+        <v>47.60334884569328</v>
       </c>
       <c r="F8" t="n">
-        <v>36.78552226746926</v>
+        <v>43.573404189341</v>
       </c>
       <c r="G8" t="n">
-        <v>9.096434129380377</v>
+        <v>39.2562002148421</v>
       </c>
       <c r="H8" t="n">
-        <v>37.33779885995996</v>
+        <v>41.23038426561097</v>
       </c>
       <c r="I8" t="n">
-        <v>42.30940799436627</v>
+        <v>44.70412634327087</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:26</t>
+          <t>2024-09-05 16:26:26</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>34.30219267017762</v>
+        <v>40.66926706667894</v>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" t="n">
-        <v>26.50350611520347</v>
+        <v>28.1802122888948</v>
       </c>
       <c r="E9" t="n">
-        <v>41.61438170584872</v>
+        <v>46.60290329155291</v>
       </c>
       <c r="F9" t="n">
-        <v>40.44579187749442</v>
+        <v>39.8784778755585</v>
       </c>
       <c r="G9" t="n">
-        <v>31.09276408894518</v>
+        <v>35.37107715053161</v>
       </c>
       <c r="H9" t="n">
-        <v>34.78098261831244</v>
-      </c>
-      <c r="I9" t="inlineStr"/>
+        <v>46.93211132070783</v>
+      </c>
+      <c r="I9" t="n">
+        <v>44.48161980008019</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:28</t>
+          <t>2024-09-05 16:26:28</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>31.4191755115896</v>
+        <v>36.89461772494965</v>
       </c>
       <c r="C10" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="n">
-        <v>29.7111132836741</v>
+        <v>16.59955536767804</v>
       </c>
       <c r="E10" t="n">
-        <v>28.62649756756432</v>
+        <v>44.04186409855882</v>
       </c>
       <c r="F10" t="n">
-        <v>31.47254824573881</v>
+        <v>36.67652033800455</v>
       </c>
       <c r="G10" t="n">
-        <v>36.97701854294326</v>
+        <v>28.37914430087582</v>
       </c>
       <c r="H10" t="n">
-        <v>31.02943311162553</v>
+        <v>46.40942613189525</v>
       </c>
       <c r="I10" t="n">
-        <v>39.63552770895878</v>
+        <v>44.43161581648308</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-09-04 22:19:30</t>
+          <t>2024-09-05 16:26:30</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>31.95574066422177</v>
+        <v>38.32191102112408</v>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D11" t="n">
-        <v>26.58838950402026</v>
+        <v>24.38172076865941</v>
       </c>
       <c r="E11" t="n">
-        <v>27.73355927719795</v>
+        <v>41.76891482328433</v>
       </c>
       <c r="F11" t="n">
-        <v>27.38921437325381</v>
+        <v>38.93729650599941</v>
       </c>
       <c r="G11" t="n">
-        <v>40.22682027771131</v>
+        <v>34.58701485230315</v>
       </c>
       <c r="H11" t="n">
-        <v>39.9352074730528</v>
+        <v>46.32581083422311</v>
       </c>
       <c r="I11" t="n">
-        <v>39.63552770895878</v>
-      </c>
+        <v>45.96939430686758</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:32</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>39.57542782684278</v>
+      </c>
+      <c r="C12" t="n">
+        <v>28</v>
+      </c>
+      <c r="D12" t="n">
+        <v>33.999518591834</v>
+      </c>
+      <c r="E12" t="n">
+        <v>40.96614660084381</v>
+      </c>
+      <c r="F12" t="n">
+        <v>42.79198247685642</v>
+      </c>
+      <c r="G12" t="n">
+        <v>40.50647329371137</v>
+      </c>
+      <c r="H12" t="n">
+        <v>36.05655715371277</v>
+      </c>
+      <c r="I12" t="n">
+        <v>45.44526039925524</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:34</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>32.04449003228069</v>
+      </c>
+      <c r="C13" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" t="n">
+        <v>36.45939547546437</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25.93781566389877</v>
+      </c>
+      <c r="F13" t="n">
+        <v>40.28381698140029</v>
+      </c>
+      <c r="G13" t="n">
+        <v>28.09491443461864</v>
+      </c>
+      <c r="H13" t="n">
+        <v>33.2266340284004</v>
+      </c>
+      <c r="I13" t="n">
+        <v>45.44526039925524</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:36</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>30.38681390948057</v>
+      </c>
+      <c r="C14" t="n">
+        <v>32</v>
+      </c>
+      <c r="D14" t="n">
+        <v>36.20502598754521</v>
+      </c>
+      <c r="E14" t="n">
+        <v>28.17900756655807</v>
+      </c>
+      <c r="F14" t="n">
+        <v>34.00307644721714</v>
+      </c>
+      <c r="G14" t="n">
+        <v>24.02072998643741</v>
+      </c>
+      <c r="H14" t="n">
+        <v>31.90171761941405</v>
+      </c>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:38</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>33.56347789332297</v>
+      </c>
+      <c r="C15" t="n">
+        <v>32</v>
+      </c>
+      <c r="D15" t="n">
+        <v>26.5759245757448</v>
+      </c>
+      <c r="E15" t="n">
+        <v>31.41435301858062</v>
+      </c>
+      <c r="F15" t="n">
+        <v>39.954554015193</v>
+      </c>
+      <c r="G15" t="n">
+        <v>32.7408007418323</v>
+      </c>
+      <c r="H15" t="n">
+        <v>39.39434642462023</v>
+      </c>
+      <c r="I15" t="n">
+        <v>28.79061259471663</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:40</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>29.59491566419853</v>
+      </c>
+      <c r="C16" t="n">
+        <v>34</v>
+      </c>
+      <c r="D16" t="n">
+        <v>34.15460631877843</v>
+      </c>
+      <c r="E16" t="n">
+        <v>22.83155189509473</v>
+      </c>
+      <c r="F16" t="n">
+        <v>29.03156229004734</v>
+      </c>
+      <c r="G16" t="n">
+        <v>23.44346783099515</v>
+      </c>
+      <c r="H16" t="n">
+        <v>42.64304956338959</v>
+      </c>
+      <c r="I16" t="n">
+        <v>40.86010412505591</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:42</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>28.20248575222477</v>
+      </c>
+      <c r="C17" t="n">
+        <v>35</v>
+      </c>
+      <c r="D17" t="n">
+        <v>27.07603603431534</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21.71989214864572</v>
+      </c>
+      <c r="F17" t="n">
+        <v>37.20545544112707</v>
+      </c>
+      <c r="G17" t="n">
+        <v>18.39827058120073</v>
+      </c>
+      <c r="H17" t="n">
+        <v>39.69526164193873</v>
+      </c>
+      <c r="I17" t="n">
+        <v>40.86649705364763</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:44</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>24.50072134283583</v>
+      </c>
+      <c r="C18" t="n">
+        <v>36</v>
+      </c>
+      <c r="D18" t="n">
+        <v>23.14772716937578</v>
+      </c>
+      <c r="E18" t="n">
+        <v>24.01554020043239</v>
+      </c>
+      <c r="F18" t="n">
+        <v>32.38643069070339</v>
+      </c>
+      <c r="G18" t="n">
+        <v>18.08215283725739</v>
+      </c>
+      <c r="H18" t="n">
+        <v>25.1490677037508</v>
+      </c>
+      <c r="I18" t="n">
+        <v>40.86649705364763</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:46</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>25.86755567995148</v>
+      </c>
+      <c r="C19" t="n">
+        <v>39</v>
+      </c>
+      <c r="D19" t="n">
+        <v>28.93038303714463</v>
+      </c>
+      <c r="E19" t="n">
+        <v>24.46591458570537</v>
+      </c>
+      <c r="F19" t="n">
+        <v>31.42114537663517</v>
+      </c>
+      <c r="G19" t="n">
+        <v>15.41103263687732</v>
+      </c>
+      <c r="H19" t="n">
+        <v>30.7735407421347</v>
+      </c>
+      <c r="I19" t="n">
+        <v>40.86649705364763</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:48</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>23.24644091634997</v>
+      </c>
+      <c r="C20" t="n">
+        <v>41</v>
+      </c>
+      <c r="D20" t="n">
+        <v>17.45384348283104</v>
+      </c>
+      <c r="E20" t="n">
+        <v>24.19667439831155</v>
+      </c>
+      <c r="F20" t="n">
+        <v>24.69714231000195</v>
+      </c>
+      <c r="G20" t="n">
+        <v>13.31433957836287</v>
+      </c>
+      <c r="H20" t="n">
+        <v>39.79712520266563</v>
+      </c>
+      <c r="I20" t="n">
+        <v>41.16854508937149</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:50</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>18.59543963463927</v>
+      </c>
+      <c r="C21" t="n">
+        <v>42</v>
+      </c>
+      <c r="D21" t="n">
+        <v>17.79097964467142</v>
+      </c>
+      <c r="E21" t="n">
+        <v>14.46553922718401</v>
+      </c>
+      <c r="F21" t="n">
+        <v>23.38156374940598</v>
+      </c>
+      <c r="G21" t="n">
+        <v>12.58385392641311</v>
+      </c>
+      <c r="H21" t="n">
+        <v>22.46041891055589</v>
+      </c>
+      <c r="I21" t="n">
+        <v>41.16854508937149</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:52</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>20.45259030265783</v>
+      </c>
+      <c r="C22" t="n">
+        <v>42</v>
+      </c>
+      <c r="D22" t="n">
+        <v>24.9958959512678</v>
+      </c>
+      <c r="E22" t="n">
+        <v>15.56001623548116</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20.53795388552441</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20.546965660764</v>
+      </c>
+      <c r="H22" t="n">
+        <v>19.67463142732815</v>
+      </c>
+      <c r="I22" t="n">
+        <v>41.47059312509535</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:54</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>20.15587089171682</v>
+      </c>
+      <c r="C23" t="n">
+        <v>42</v>
+      </c>
+      <c r="D23" t="n">
+        <v>13.80673568084719</v>
+      </c>
+      <c r="E23" t="n">
+        <v>17.24954869044628</v>
+      </c>
+      <c r="F23" t="n">
+        <v>14.70211328579419</v>
+      </c>
+      <c r="G23" t="n">
+        <v>26.62659045390801</v>
+      </c>
+      <c r="H23" t="n">
+        <v>21.62647999132364</v>
+      </c>
+      <c r="I23" t="n">
+        <v>41.47059312509535</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:56</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>16.15076761667705</v>
+      </c>
+      <c r="C24" t="n">
+        <v>42</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7.013145099799249</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10.00303143767264</v>
+      </c>
+      <c r="F24" t="n">
+        <v>8.662532029887458</v>
+      </c>
+      <c r="G24" t="n">
+        <v>19.99678125429856</v>
+      </c>
+      <c r="H24" t="n">
+        <v>29.97425114966626</v>
+      </c>
+      <c r="I24" t="n">
+        <v>41.47059312509535</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:26:58</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>9.837668677985929</v>
+      </c>
+      <c r="C25" t="n">
+        <v>43</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>8.236463511673685</v>
+      </c>
+      <c r="F25" t="n">
+        <v>7.507956462918094</v>
+      </c>
+      <c r="G25" t="n">
+        <v>12.1822277050365</v>
+      </c>
+      <c r="H25" t="n">
+        <v>13.63184154909024</v>
+      </c>
+      <c r="I25" t="n">
+        <v>41.47059312509535</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:00</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>7.359873069444943</v>
+      </c>
+      <c r="C26" t="n">
+        <v>45</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>4.007793006542574</v>
+      </c>
+      <c r="F26" t="n">
+        <v>6.901357070134914</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.718073178006484</v>
+      </c>
+      <c r="H26" t="n">
+        <v>15.80176018323224</v>
+      </c>
+      <c r="I26" t="n">
+        <v>41.47059312509535</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:02</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>6.31729282229663</v>
+      </c>
+      <c r="C27" t="n">
+        <v>45</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7.133708342272286</v>
+      </c>
+      <c r="F27" t="n">
+        <v>6.178490696654769</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.577763083429367e-08</v>
+      </c>
+      <c r="H27" t="n">
+        <v>15.68409168635296</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:04</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3.431673803270295</v>
+      </c>
+      <c r="C28" t="n">
+        <v>45</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.834527567092323</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.254557833653952e-08</v>
+      </c>
+      <c r="H28" t="n">
+        <v>11.19354834249055</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:06</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2.972286206099517</v>
+      </c>
+      <c r="C29" t="n">
+        <v>47</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.069061168043947</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.019442224552366e-08</v>
+      </c>
+      <c r="H29" t="n">
+        <v>9.366153406407387</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:08</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1.829039528020951</v>
+      </c>
+      <c r="C30" t="n">
+        <v>47</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2.918428346989492</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>8.627594581429778e-09</v>
+      </c>
+      <c r="H30" t="n">
+        <v>4.218843252586639</v>
+      </c>
+      <c r="I30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:10</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1.762050761974766</v>
+      </c>
+      <c r="C31" t="n">
+        <v>48</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4.247450243844938e-09</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>7.488980404284728e-09</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7.688948766926111</v>
+      </c>
+      <c r="I31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:13</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.9893470063994662</v>
+      </c>
+      <c r="C32" t="n">
+        <v>48</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.826481387777429e-09</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6.707496076636361e-09</v>
+      </c>
+      <c r="H32" t="n">
+        <v>4.317150562063836</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:15</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2.396045138255164e-09</v>
+      </c>
+      <c r="C33" t="n">
+        <v>48</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.54304974164563e-09</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>6.186442051156343e-09</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:17</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2.205871217757892e-09</v>
+      </c>
+      <c r="C34" t="n">
+        <v>48</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3.268455023783986e-09</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>5.685499309561901e-09</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:19</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2.027995647834409e-09</v>
+      </c>
+      <c r="C35" t="n">
+        <v>48</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.010587970873156e-09</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>5.21849715329543e-09</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-09-05 16:27:21</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1.871699221538834e-09</v>
+      </c>
+      <c r="C36" t="n">
+        <v>48</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.78318189135163e-09</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>4.809383426358961e-09</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>